<commit_message>
iteration working, need to get constraints to update in loop
</commit_message>
<xml_diff>
--- a/DCA-DCM Constraints.xlsx
+++ b/DCA-DCM Constraints.xlsx
@@ -1035,8 +1035,8 @@
   <dimension ref="A1:AF169"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A139" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA147" sqref="AA147"/>
+      <pane ySplit="9" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="X169" sqref="X169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1422,7 +1422,7 @@
         <v>0</v>
       </c>
       <c r="AF10" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1520,7 +1520,7 @@
         <v>0</v>
       </c>
       <c r="AF11" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2304,7 +2304,7 @@
         <v>0</v>
       </c>
       <c r="AF19" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2402,7 +2402,7 @@
         <v>0</v>
       </c>
       <c r="AF20" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2598,7 +2598,7 @@
         <v>0</v>
       </c>
       <c r="AF22" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2696,7 +2696,7 @@
         <v>0</v>
       </c>
       <c r="AF23" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2892,7 +2892,7 @@
         <v>0</v>
       </c>
       <c r="AF25" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3480,7 +3480,7 @@
         <v>0</v>
       </c>
       <c r="AF31" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3578,7 +3578,7 @@
         <v>0</v>
       </c>
       <c r="AF32" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3676,188 +3676,498 @@
         <v>0</v>
       </c>
       <c r="AF33" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="9"/>
-      <c r="I34" s="9"/>
-      <c r="J34" s="9"/>
-      <c r="K34" s="9"/>
-      <c r="L34" s="9"/>
-      <c r="M34" s="9"/>
-      <c r="N34" s="9"/>
-      <c r="O34" s="9"/>
-      <c r="P34" s="9"/>
-      <c r="Q34" s="9"/>
-      <c r="R34" s="9"/>
-      <c r="S34" s="9"/>
-      <c r="T34" s="9"/>
-      <c r="U34" s="9"/>
-      <c r="V34" s="9"/>
-      <c r="W34" s="9"/>
-      <c r="X34" s="9"/>
-      <c r="Y34" s="9"/>
-      <c r="Z34" s="9"/>
-      <c r="AA34" s="9"/>
-      <c r="AB34" s="9"/>
-      <c r="AC34" s="9"/>
-      <c r="AD34" s="9"/>
-      <c r="AE34" s="9"/>
-      <c r="AF34" s="9"/>
+      <c r="B34" s="9">
+        <v>1</v>
+      </c>
+      <c r="C34" s="9">
+        <v>0</v>
+      </c>
+      <c r="D34" s="9">
+        <v>0</v>
+      </c>
+      <c r="E34" s="9">
+        <v>0</v>
+      </c>
+      <c r="F34" s="9">
+        <v>1</v>
+      </c>
+      <c r="G34" s="9">
+        <v>1</v>
+      </c>
+      <c r="H34" s="9">
+        <v>1</v>
+      </c>
+      <c r="I34" s="9">
+        <v>1</v>
+      </c>
+      <c r="J34" s="9">
+        <v>1</v>
+      </c>
+      <c r="K34" s="9">
+        <v>1</v>
+      </c>
+      <c r="L34" s="9">
+        <v>1</v>
+      </c>
+      <c r="M34" s="9">
+        <v>1</v>
+      </c>
+      <c r="N34" s="9">
+        <v>1</v>
+      </c>
+      <c r="O34" s="9">
+        <v>1</v>
+      </c>
+      <c r="P34" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q34" s="9">
+        <v>1</v>
+      </c>
+      <c r="R34" s="9">
+        <v>1</v>
+      </c>
+      <c r="S34" s="9">
+        <v>1</v>
+      </c>
+      <c r="T34" s="9">
+        <v>1</v>
+      </c>
+      <c r="U34" s="9">
+        <v>1</v>
+      </c>
+      <c r="V34" s="9">
+        <v>1</v>
+      </c>
+      <c r="W34" s="9">
+        <v>1</v>
+      </c>
+      <c r="X34" s="9">
+        <v>1</v>
+      </c>
+      <c r="Y34" s="9">
+        <v>1</v>
+      </c>
+      <c r="Z34" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA34" s="9">
+        <v>1</v>
+      </c>
+      <c r="AB34" s="9">
+        <v>1</v>
+      </c>
+      <c r="AC34" s="9">
+        <v>1</v>
+      </c>
+      <c r="AD34" s="9">
+        <v>1</v>
+      </c>
+      <c r="AE34" s="9">
+        <v>1</v>
+      </c>
+      <c r="AF34" s="9">
+        <v>1</v>
+      </c>
     </row>
     <row r="35" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="B35" s="9"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="9"/>
-      <c r="J35" s="9"/>
-      <c r="K35" s="9"/>
-      <c r="L35" s="9"/>
-      <c r="M35" s="9"/>
-      <c r="N35" s="9"/>
-      <c r="O35" s="9"/>
-      <c r="P35" s="9"/>
-      <c r="Q35" s="9"/>
-      <c r="R35" s="9"/>
-      <c r="S35" s="9"/>
-      <c r="T35" s="9"/>
-      <c r="U35" s="9"/>
-      <c r="V35" s="9"/>
-      <c r="W35" s="9"/>
-      <c r="X35" s="9"/>
-      <c r="Y35" s="9"/>
-      <c r="Z35" s="9"/>
-      <c r="AA35" s="9"/>
-      <c r="AB35" s="9"/>
-      <c r="AC35" s="9"/>
-      <c r="AD35" s="9"/>
-      <c r="AE35" s="9"/>
-      <c r="AF35" s="9"/>
+      <c r="B35" s="9">
+        <v>1</v>
+      </c>
+      <c r="C35" s="9">
+        <v>0</v>
+      </c>
+      <c r="D35" s="9">
+        <v>0</v>
+      </c>
+      <c r="E35" s="9">
+        <v>0</v>
+      </c>
+      <c r="F35" s="9">
+        <v>1</v>
+      </c>
+      <c r="G35" s="9">
+        <v>1</v>
+      </c>
+      <c r="H35" s="9">
+        <v>1</v>
+      </c>
+      <c r="I35" s="9">
+        <v>1</v>
+      </c>
+      <c r="J35" s="9">
+        <v>1</v>
+      </c>
+      <c r="K35" s="9">
+        <v>1</v>
+      </c>
+      <c r="L35" s="9">
+        <v>1</v>
+      </c>
+      <c r="M35" s="9">
+        <v>1</v>
+      </c>
+      <c r="N35" s="9">
+        <v>1</v>
+      </c>
+      <c r="O35" s="9">
+        <v>1</v>
+      </c>
+      <c r="P35" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q35" s="9">
+        <v>1</v>
+      </c>
+      <c r="R35" s="9">
+        <v>1</v>
+      </c>
+      <c r="S35" s="9">
+        <v>1</v>
+      </c>
+      <c r="T35" s="9">
+        <v>1</v>
+      </c>
+      <c r="U35" s="9">
+        <v>1</v>
+      </c>
+      <c r="V35" s="9">
+        <v>1</v>
+      </c>
+      <c r="W35" s="9">
+        <v>1</v>
+      </c>
+      <c r="X35" s="9">
+        <v>1</v>
+      </c>
+      <c r="Y35" s="9">
+        <v>1</v>
+      </c>
+      <c r="Z35" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA35" s="9">
+        <v>1</v>
+      </c>
+      <c r="AB35" s="9">
+        <v>1</v>
+      </c>
+      <c r="AC35" s="9">
+        <v>1</v>
+      </c>
+      <c r="AD35" s="9">
+        <v>1</v>
+      </c>
+      <c r="AE35" s="9">
+        <v>1</v>
+      </c>
+      <c r="AF35" s="9">
+        <v>1</v>
+      </c>
     </row>
     <row r="36" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="B36" s="9"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="9"/>
-      <c r="H36" s="9"/>
-      <c r="I36" s="9"/>
-      <c r="J36" s="9"/>
-      <c r="K36" s="9"/>
-      <c r="L36" s="9"/>
-      <c r="M36" s="9"/>
-      <c r="N36" s="9"/>
-      <c r="O36" s="9"/>
-      <c r="P36" s="9"/>
-      <c r="Q36" s="9"/>
-      <c r="R36" s="9"/>
-      <c r="S36" s="9"/>
-      <c r="T36" s="9"/>
-      <c r="U36" s="9"/>
-      <c r="V36" s="9"/>
-      <c r="W36" s="9"/>
-      <c r="X36" s="9"/>
-      <c r="Y36" s="9"/>
-      <c r="Z36" s="9"/>
-      <c r="AA36" s="9"/>
-      <c r="AB36" s="9"/>
-      <c r="AC36" s="9"/>
-      <c r="AD36" s="9"/>
-      <c r="AE36" s="9"/>
-      <c r="AF36" s="9"/>
+      <c r="B36" s="9">
+        <v>0</v>
+      </c>
+      <c r="C36" s="9">
+        <v>0</v>
+      </c>
+      <c r="D36" s="9">
+        <v>0</v>
+      </c>
+      <c r="E36" s="9">
+        <v>0</v>
+      </c>
+      <c r="F36" s="9">
+        <v>0</v>
+      </c>
+      <c r="G36" s="9">
+        <v>0</v>
+      </c>
+      <c r="H36" s="9">
+        <v>0</v>
+      </c>
+      <c r="I36" s="9">
+        <v>0</v>
+      </c>
+      <c r="J36" s="9">
+        <v>0</v>
+      </c>
+      <c r="K36" s="9">
+        <v>0</v>
+      </c>
+      <c r="L36" s="9">
+        <v>0</v>
+      </c>
+      <c r="M36" s="9">
+        <v>0</v>
+      </c>
+      <c r="N36" s="9">
+        <v>0</v>
+      </c>
+      <c r="O36" s="9">
+        <v>0</v>
+      </c>
+      <c r="P36" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="9">
+        <v>0</v>
+      </c>
+      <c r="R36" s="9">
+        <v>0</v>
+      </c>
+      <c r="S36" s="9">
+        <v>0</v>
+      </c>
+      <c r="T36" s="9">
+        <v>0</v>
+      </c>
+      <c r="U36" s="9">
+        <v>0</v>
+      </c>
+      <c r="V36" s="9">
+        <v>0</v>
+      </c>
+      <c r="W36" s="9">
+        <v>0</v>
+      </c>
+      <c r="X36" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y36" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z36" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA36" s="9">
+        <v>1</v>
+      </c>
+      <c r="AB36" s="9">
+        <v>1</v>
+      </c>
+      <c r="AC36" s="9">
+        <v>1</v>
+      </c>
+      <c r="AD36" s="9">
+        <v>1</v>
+      </c>
+      <c r="AE36" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF36" s="9">
+        <v>1</v>
+      </c>
     </row>
     <row r="37" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="B37" s="11"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="11"/>
-      <c r="K37" s="11"/>
-      <c r="L37" s="11"/>
-      <c r="M37" s="11"/>
-      <c r="N37" s="11"/>
-      <c r="O37" s="11"/>
-      <c r="P37" s="11"/>
-      <c r="Q37" s="11"/>
-      <c r="R37" s="11"/>
-      <c r="S37" s="11"/>
-      <c r="T37" s="11"/>
-      <c r="U37" s="11"/>
-      <c r="V37" s="11"/>
-      <c r="W37" s="11"/>
-      <c r="X37" s="11"/>
-      <c r="Y37" s="11"/>
-      <c r="Z37" s="11"/>
-      <c r="AA37" s="11"/>
-      <c r="AB37" s="11"/>
-      <c r="AC37" s="11"/>
-      <c r="AD37" s="11"/>
-      <c r="AE37" s="11"/>
-      <c r="AF37" s="11"/>
+      <c r="B37" s="11">
+        <v>0</v>
+      </c>
+      <c r="C37" s="11">
+        <v>0</v>
+      </c>
+      <c r="D37" s="11">
+        <v>0</v>
+      </c>
+      <c r="E37" s="11">
+        <v>0</v>
+      </c>
+      <c r="F37" s="11">
+        <v>0</v>
+      </c>
+      <c r="G37" s="11">
+        <v>0</v>
+      </c>
+      <c r="H37" s="11">
+        <v>0</v>
+      </c>
+      <c r="I37" s="11">
+        <v>0</v>
+      </c>
+      <c r="J37" s="11">
+        <v>0</v>
+      </c>
+      <c r="K37" s="11">
+        <v>0</v>
+      </c>
+      <c r="L37" s="11">
+        <v>0</v>
+      </c>
+      <c r="M37" s="11">
+        <v>0</v>
+      </c>
+      <c r="N37" s="11">
+        <v>0</v>
+      </c>
+      <c r="O37" s="11">
+        <v>0</v>
+      </c>
+      <c r="P37" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="11">
+        <v>0</v>
+      </c>
+      <c r="R37" s="11">
+        <v>0</v>
+      </c>
+      <c r="S37" s="11">
+        <v>0</v>
+      </c>
+      <c r="T37" s="11">
+        <v>0</v>
+      </c>
+      <c r="U37" s="11">
+        <v>0</v>
+      </c>
+      <c r="V37" s="11">
+        <v>0</v>
+      </c>
+      <c r="W37" s="11">
+        <v>0</v>
+      </c>
+      <c r="X37" s="11">
+        <v>0</v>
+      </c>
+      <c r="Y37" s="11">
+        <v>0</v>
+      </c>
+      <c r="Z37" s="11">
+        <v>0</v>
+      </c>
+      <c r="AA37" s="11">
+        <v>0</v>
+      </c>
+      <c r="AB37" s="11">
+        <v>1</v>
+      </c>
+      <c r="AC37" s="11">
+        <v>0</v>
+      </c>
+      <c r="AD37" s="11">
+        <v>0</v>
+      </c>
+      <c r="AE37" s="11">
+        <v>0</v>
+      </c>
+      <c r="AF37" s="11">
+        <v>0</v>
+      </c>
     </row>
     <row r="38" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B38" s="11"/>
-      <c r="C38" s="11"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="11"/>
-      <c r="I38" s="11"/>
-      <c r="J38" s="11"/>
-      <c r="K38" s="11"/>
-      <c r="L38" s="11"/>
-      <c r="M38" s="11"/>
-      <c r="N38" s="11"/>
-      <c r="O38" s="11"/>
-      <c r="P38" s="11"/>
-      <c r="Q38" s="11"/>
-      <c r="R38" s="11"/>
-      <c r="S38" s="11"/>
-      <c r="T38" s="11"/>
-      <c r="U38" s="11"/>
-      <c r="V38" s="11"/>
-      <c r="W38" s="11"/>
-      <c r="X38" s="11"/>
-      <c r="Y38" s="11"/>
-      <c r="Z38" s="11"/>
-      <c r="AA38" s="11"/>
-      <c r="AB38" s="11"/>
-      <c r="AC38" s="11"/>
-      <c r="AD38" s="11"/>
-      <c r="AE38" s="11"/>
-      <c r="AF38" s="11"/>
+      <c r="B38" s="11">
+        <v>0</v>
+      </c>
+      <c r="C38" s="11">
+        <v>0</v>
+      </c>
+      <c r="D38" s="11">
+        <v>0</v>
+      </c>
+      <c r="E38" s="11">
+        <v>0</v>
+      </c>
+      <c r="F38" s="11">
+        <v>0</v>
+      </c>
+      <c r="G38" s="11">
+        <v>0</v>
+      </c>
+      <c r="H38" s="11">
+        <v>0</v>
+      </c>
+      <c r="I38" s="11">
+        <v>0</v>
+      </c>
+      <c r="J38" s="11">
+        <v>0</v>
+      </c>
+      <c r="K38" s="11">
+        <v>0</v>
+      </c>
+      <c r="L38" s="11">
+        <v>0</v>
+      </c>
+      <c r="M38" s="11">
+        <v>0</v>
+      </c>
+      <c r="N38" s="11">
+        <v>0</v>
+      </c>
+      <c r="O38" s="11">
+        <v>0</v>
+      </c>
+      <c r="P38" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q38" s="11">
+        <v>0</v>
+      </c>
+      <c r="R38" s="11">
+        <v>0</v>
+      </c>
+      <c r="S38" s="11">
+        <v>0</v>
+      </c>
+      <c r="T38" s="11">
+        <v>0</v>
+      </c>
+      <c r="U38" s="11">
+        <v>0</v>
+      </c>
+      <c r="V38" s="11">
+        <v>0</v>
+      </c>
+      <c r="W38" s="11">
+        <v>0</v>
+      </c>
+      <c r="X38" s="11">
+        <v>0</v>
+      </c>
+      <c r="Y38" s="11">
+        <v>0</v>
+      </c>
+      <c r="Z38" s="11">
+        <v>1</v>
+      </c>
+      <c r="AA38" s="11">
+        <v>0</v>
+      </c>
+      <c r="AB38" s="11">
+        <v>0</v>
+      </c>
+      <c r="AC38" s="11">
+        <v>0</v>
+      </c>
+      <c r="AD38" s="11">
+        <v>0</v>
+      </c>
+      <c r="AE38" s="11">
+        <v>0</v>
+      </c>
+      <c r="AF38" s="11">
+        <v>0</v>
+      </c>
     </row>
     <row r="39" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
@@ -3954,7 +4264,7 @@
         <v>0</v>
       </c>
       <c r="AF39" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4052,7 +4362,7 @@
         <v>0</v>
       </c>
       <c r="AF40" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4248,7 +4558,7 @@
         <v>0</v>
       </c>
       <c r="AF42" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4836,7 +5146,7 @@
         <v>0</v>
       </c>
       <c r="AF48" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4934,7 +5244,7 @@
         <v>0</v>
       </c>
       <c r="AF49" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5032,7 +5342,7 @@
         <v>0</v>
       </c>
       <c r="AF50" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5130,7 +5440,7 @@
         <v>0</v>
       </c>
       <c r="AF51" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5228,7 +5538,7 @@
         <v>0</v>
       </c>
       <c r="AF52" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5424,7 +5734,7 @@
         <v>0</v>
       </c>
       <c r="AF54" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6012,7 +6322,7 @@
         <v>0</v>
       </c>
       <c r="AF60" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6306,7 +6616,7 @@
         <v>0</v>
       </c>
       <c r="AF63" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6404,7 +6714,7 @@
         <v>0</v>
       </c>
       <c r="AF64" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6412,7 +6722,7 @@
         <v>86</v>
       </c>
       <c r="B65" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C65" s="9">
         <v>0</v>
@@ -6502,7 +6812,7 @@
         <v>0</v>
       </c>
       <c r="AF65" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6510,7 +6820,7 @@
         <v>87</v>
       </c>
       <c r="B66" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C66" s="9">
         <v>0</v>
@@ -6600,7 +6910,7 @@
         <v>0</v>
       </c>
       <c r="AF66" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6705,73 +7015,197 @@
       <c r="A68" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="B68" s="9"/>
-      <c r="C68" s="9"/>
-      <c r="D68" s="9"/>
-      <c r="E68" s="9"/>
-      <c r="F68" s="9"/>
-      <c r="G68" s="9"/>
-      <c r="H68" s="9"/>
-      <c r="I68" s="9"/>
-      <c r="J68" s="9"/>
-      <c r="K68" s="9"/>
-      <c r="L68" s="9"/>
-      <c r="M68" s="9"/>
-      <c r="N68" s="9"/>
-      <c r="O68" s="9"/>
-      <c r="P68" s="9"/>
-      <c r="Q68" s="9"/>
-      <c r="R68" s="9"/>
-      <c r="S68" s="9"/>
-      <c r="T68" s="9"/>
-      <c r="U68" s="9"/>
-      <c r="V68" s="9"/>
-      <c r="W68" s="9"/>
-      <c r="X68" s="9"/>
-      <c r="Y68" s="9"/>
-      <c r="Z68" s="9"/>
-      <c r="AA68" s="9"/>
-      <c r="AB68" s="9"/>
-      <c r="AC68" s="9"/>
-      <c r="AD68" s="9"/>
-      <c r="AE68" s="9"/>
-      <c r="AF68" s="9"/>
+      <c r="B68" s="9">
+        <v>0</v>
+      </c>
+      <c r="C68" s="9">
+        <v>0</v>
+      </c>
+      <c r="D68" s="9">
+        <v>0</v>
+      </c>
+      <c r="E68" s="9">
+        <v>0</v>
+      </c>
+      <c r="F68" s="9">
+        <v>0</v>
+      </c>
+      <c r="G68" s="9">
+        <v>0</v>
+      </c>
+      <c r="H68" s="9">
+        <v>0</v>
+      </c>
+      <c r="I68" s="9">
+        <v>0</v>
+      </c>
+      <c r="J68" s="9">
+        <v>0</v>
+      </c>
+      <c r="K68" s="9">
+        <v>0</v>
+      </c>
+      <c r="L68" s="9">
+        <v>1</v>
+      </c>
+      <c r="M68" s="9">
+        <v>1</v>
+      </c>
+      <c r="N68" s="9">
+        <v>0</v>
+      </c>
+      <c r="O68" s="9">
+        <v>0</v>
+      </c>
+      <c r="P68" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q68" s="9">
+        <v>0</v>
+      </c>
+      <c r="R68" s="9">
+        <v>0</v>
+      </c>
+      <c r="S68" s="9">
+        <v>0</v>
+      </c>
+      <c r="T68" s="9">
+        <v>0</v>
+      </c>
+      <c r="U68" s="9">
+        <v>1</v>
+      </c>
+      <c r="V68" s="9">
+        <v>0</v>
+      </c>
+      <c r="W68" s="9">
+        <v>0</v>
+      </c>
+      <c r="X68" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y68" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z68" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA68" s="9">
+        <v>1</v>
+      </c>
+      <c r="AB68" s="9">
+        <v>1</v>
+      </c>
+      <c r="AC68" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD68" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE68" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF68" s="9">
+        <v>1</v>
+      </c>
     </row>
     <row r="69" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="B69" s="9"/>
-      <c r="C69" s="9"/>
-      <c r="D69" s="9"/>
-      <c r="E69" s="9"/>
-      <c r="F69" s="9"/>
-      <c r="G69" s="9"/>
-      <c r="H69" s="9"/>
-      <c r="I69" s="9"/>
-      <c r="J69" s="9"/>
-      <c r="K69" s="9"/>
-      <c r="L69" s="9"/>
-      <c r="M69" s="9"/>
-      <c r="N69" s="9"/>
-      <c r="O69" s="9"/>
-      <c r="P69" s="9"/>
-      <c r="Q69" s="9"/>
-      <c r="R69" s="9"/>
-      <c r="S69" s="9"/>
-      <c r="T69" s="9"/>
-      <c r="U69" s="9"/>
-      <c r="V69" s="9"/>
-      <c r="W69" s="9"/>
-      <c r="X69" s="9"/>
-      <c r="Y69" s="9"/>
-      <c r="Z69" s="9"/>
-      <c r="AA69" s="9"/>
-      <c r="AB69" s="9"/>
-      <c r="AC69" s="9"/>
-      <c r="AD69" s="9"/>
-      <c r="AE69" s="9"/>
-      <c r="AF69" s="9"/>
+      <c r="B69" s="9">
+        <v>0</v>
+      </c>
+      <c r="C69" s="9">
+        <v>0</v>
+      </c>
+      <c r="D69" s="9">
+        <v>0</v>
+      </c>
+      <c r="E69" s="9">
+        <v>1</v>
+      </c>
+      <c r="F69" s="9">
+        <v>0</v>
+      </c>
+      <c r="G69" s="9">
+        <v>0</v>
+      </c>
+      <c r="H69" s="9">
+        <v>0</v>
+      </c>
+      <c r="I69" s="9">
+        <v>0</v>
+      </c>
+      <c r="J69" s="9">
+        <v>0</v>
+      </c>
+      <c r="K69" s="9">
+        <v>0</v>
+      </c>
+      <c r="L69" s="9">
+        <v>0</v>
+      </c>
+      <c r="M69" s="9">
+        <v>0</v>
+      </c>
+      <c r="N69" s="9">
+        <v>0</v>
+      </c>
+      <c r="O69" s="9">
+        <v>1</v>
+      </c>
+      <c r="P69" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q69" s="9">
+        <v>0</v>
+      </c>
+      <c r="R69" s="9">
+        <v>0</v>
+      </c>
+      <c r="S69" s="9">
+        <v>0</v>
+      </c>
+      <c r="T69" s="9">
+        <v>0</v>
+      </c>
+      <c r="U69" s="9">
+        <v>0</v>
+      </c>
+      <c r="V69" s="9">
+        <v>0</v>
+      </c>
+      <c r="W69" s="9">
+        <v>0</v>
+      </c>
+      <c r="X69" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y69" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z69" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA69" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB69" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC69" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD69" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE69" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF69" s="9">
+        <v>1</v>
+      </c>
     </row>
     <row r="70" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="10" t="s">
@@ -6966,7 +7400,7 @@
         <v>0</v>
       </c>
       <c r="AF71" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7162,7 +7596,7 @@
         <v>0</v>
       </c>
       <c r="AF73" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7750,7 +8184,7 @@
         <v>0</v>
       </c>
       <c r="AF79" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8730,7 +9164,7 @@
         <v>0</v>
       </c>
       <c r="AF89" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8828,7 +9262,7 @@
         <v>0</v>
       </c>
       <c r="AF90" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8926,7 +9360,7 @@
         <v>0</v>
       </c>
       <c r="AF91" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8934,7 +9368,7 @@
         <v>113</v>
       </c>
       <c r="B92" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C92" s="9">
         <v>0</v>
@@ -8943,7 +9377,7 @@
         <v>0</v>
       </c>
       <c r="E92" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F92" s="9">
         <v>0</v>
@@ -9024,7 +9458,7 @@
         <v>0</v>
       </c>
       <c r="AF92" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9032,7 +9466,7 @@
         <v>114</v>
       </c>
       <c r="B93" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C93" s="9">
         <v>0</v>
@@ -9041,7 +9475,7 @@
         <v>0</v>
       </c>
       <c r="E93" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F93" s="9">
         <v>0</v>
@@ -9122,7 +9556,7 @@
         <v>0</v>
       </c>
       <c r="AF93" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9318,7 +9752,7 @@
         <v>0</v>
       </c>
       <c r="AF95" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9612,7 +10046,7 @@
         <v>0</v>
       </c>
       <c r="AF98" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9710,7 +10144,7 @@
         <v>0</v>
       </c>
       <c r="AF99" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9808,7 +10242,7 @@
         <v>0</v>
       </c>
       <c r="AF100" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9906,7 +10340,7 @@
         <v>0</v>
       </c>
       <c r="AF101" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10004,7 +10438,7 @@
         <v>0</v>
       </c>
       <c r="AF102" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10102,7 +10536,7 @@
         <v>0</v>
       </c>
       <c r="AF103" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10200,7 +10634,7 @@
         <v>0</v>
       </c>
       <c r="AF104" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10298,7 +10732,7 @@
         <v>0</v>
       </c>
       <c r="AF105" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="106" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10396,7 +10830,7 @@
         <v>0</v>
       </c>
       <c r="AF106" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10494,7 +10928,7 @@
         <v>0</v>
       </c>
       <c r="AF107" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="108" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10592,7 +11026,7 @@
         <v>0</v>
       </c>
       <c r="AF108" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10690,7 +11124,7 @@
         <v>0</v>
       </c>
       <c r="AF109" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="110" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10788,7 +11222,7 @@
         <v>0</v>
       </c>
       <c r="AF110" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="111" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10886,7 +11320,7 @@
         <v>0</v>
       </c>
       <c r="AF111" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10984,7 +11418,7 @@
         <v>0</v>
       </c>
       <c r="AF112" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="113" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11082,7 +11516,7 @@
         <v>0</v>
       </c>
       <c r="AF113" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11180,7 +11614,7 @@
         <v>0</v>
       </c>
       <c r="AF114" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="115" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11278,7 +11712,7 @@
         <v>0</v>
       </c>
       <c r="AF115" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="116" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11376,7 +11810,7 @@
         <v>0</v>
       </c>
       <c r="AF116" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="117" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11474,7 +11908,7 @@
         <v>0</v>
       </c>
       <c r="AF117" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="118" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11572,7 +12006,7 @@
         <v>0</v>
       </c>
       <c r="AF118" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="119" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11670,7 +12104,7 @@
         <v>0</v>
       </c>
       <c r="AF119" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="120" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11768,7 +12202,7 @@
         <v>0</v>
       </c>
       <c r="AF120" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="121" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11866,7 +12300,7 @@
         <v>0</v>
       </c>
       <c r="AF121" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11964,7 +12398,7 @@
         <v>0</v>
       </c>
       <c r="AF122" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="123" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12062,7 +12496,7 @@
         <v>0</v>
       </c>
       <c r="AF123" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="124" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12160,7 +12594,7 @@
         <v>0</v>
       </c>
       <c r="AF124" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="125" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12258,7 +12692,7 @@
         <v>0</v>
       </c>
       <c r="AF125" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="126" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12356,7 +12790,7 @@
         <v>0</v>
       </c>
       <c r="AF126" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="127" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12454,7 +12888,7 @@
         <v>0</v>
       </c>
       <c r="AF127" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="128" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12552,7 +12986,7 @@
         <v>0</v>
       </c>
       <c r="AF128" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="129" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12650,7 +13084,7 @@
         <v>0</v>
       </c>
       <c r="AF129" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="130" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12748,7 +13182,7 @@
         <v>0</v>
       </c>
       <c r="AF130" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="131" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12846,7 +13280,7 @@
         <v>0</v>
       </c>
       <c r="AF131" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12944,7 +13378,7 @@
         <v>0</v>
       </c>
       <c r="AF132" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="133" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13042,7 +13476,7 @@
         <v>0</v>
       </c>
       <c r="AF133" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="134" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13140,7 +13574,7 @@
         <v>0</v>
       </c>
       <c r="AF134" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="135" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13238,7 +13672,7 @@
         <v>0</v>
       </c>
       <c r="AF135" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="136" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13336,7 +13770,7 @@
         <v>0</v>
       </c>
       <c r="AF136" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="137" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13434,7 +13868,7 @@
         <v>0</v>
       </c>
       <c r="AF137" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="138" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13532,7 +13966,7 @@
         <v>0</v>
       </c>
       <c r="AF138" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="139" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13630,7 +14064,7 @@
         <v>0</v>
       </c>
       <c r="AF139" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="140" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13728,7 +14162,7 @@
         <v>0</v>
       </c>
       <c r="AF140" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="141" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13826,7 +14260,7 @@
         <v>0</v>
       </c>
       <c r="AF141" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="142" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13924,7 +14358,7 @@
         <v>0</v>
       </c>
       <c r="AF142" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="143" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -14022,7 +14456,7 @@
         <v>0</v>
       </c>
       <c r="AF143" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="144" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -14120,7 +14554,7 @@
         <v>0</v>
       </c>
       <c r="AF144" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -14218,7 +14652,7 @@
         <v>0</v>
       </c>
       <c r="AF145" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="146" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -14316,7 +14750,7 @@
         <v>0</v>
       </c>
       <c r="AF146" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="147" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -14414,7 +14848,7 @@
         <v>0</v>
       </c>
       <c r="AF147" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="148" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -14512,7 +14946,7 @@
         <v>0</v>
       </c>
       <c r="AF148" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="149" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -14610,7 +15044,7 @@
         <v>0</v>
       </c>
       <c r="AF149" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="150" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -14708,7 +15142,7 @@
         <v>0</v>
       </c>
       <c r="AF150" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="151" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -15892,7 +16326,7 @@
         <v>184</v>
       </c>
       <c r="B163" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C163" s="11">
         <v>0</v>
@@ -15904,13 +16338,13 @@
         <v>0</v>
       </c>
       <c r="F163" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G163" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H163" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I163" s="11">
         <v>0</v>
@@ -16382,7 +16816,7 @@
         <v>189</v>
       </c>
       <c r="B168" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C168" s="11">
         <v>0</v>
@@ -16454,10 +16888,10 @@
         <v>0</v>
       </c>
       <c r="Z168" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA168" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB168" s="11">
         <v>0</v>
@@ -16528,19 +16962,19 @@
         <v>0</v>
       </c>
       <c r="R169" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S169" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T169" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U169" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V169" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W169" s="11">
         <v>0</v>

</xml_diff>

<commit_message>
changed how factor tables are used to account for custom habitat and water values
</commit_message>
<xml_diff>
--- a/DCA-DCM Constraints.xlsx
+++ b/DCA-DCM Constraints.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Manual Scenario" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="145621" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -1111,7 +1111,7 @@
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="AI160" sqref="AI160"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>